<commit_message>
modify data augmentation code and figures
</commit_message>
<xml_diff>
--- a/aug_pc_result/2026_Feb_12_20_14_09_d_separation_spearman_pc_gt_graph_AdaSyn_20_640076/aug_pc_eval_res.xlsx
+++ b/aug_pc_result/2026_Feb_12_20_14_09_d_separation_spearman_pc_gt_graph_AdaSyn_20_640076/aug_pc_eval_res.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29725"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -846,8 +846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="Z2" sqref="A2:Z9"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>

</xml_diff>